<commit_message>
add missing LCSC Part #
</commit_message>
<xml_diff>
--- a/bom/TTester-BOM_JLCSMT.xlsx
+++ b/bom/TTester-BOM_JLCSMT.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="122">
   <si>
     <t>Comment</t>
   </si>
@@ -161,22 +161,25 @@
     <t>R21</t>
   </si>
   <si>
+    <t>C26010</t>
+  </si>
+  <si>
+    <t>33k</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
     <t>C17633</t>
   </si>
   <si>
-    <t>33k</t>
-  </si>
-  <si>
-    <t>R20</t>
+    <t>3k3 0.1%</t>
+  </si>
+  <si>
+    <t>R19</t>
   </si>
   <si>
     <t>C2989690</t>
-  </si>
-  <si>
-    <t>3k3 0.1%</t>
-  </si>
-  <si>
-    <t>R19</t>
   </si>
   <si>
     <t>10k 0.1%</t>
@@ -1091,329 +1094,329 @@
         <v>29</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="A26" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="A27" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" ht="13.5" customHeight="1">
       <c r="A28" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="A29" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" ht="13.5" customHeight="1">
       <c r="A30" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1">
       <c r="A31" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="A32" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="A33" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="A34" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="A35" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" ht="13.5" customHeight="1">

</xml_diff>